<commit_message>
Remove empty from data tabel and add null-objects
</commit_message>
<xml_diff>
--- a/priv/repo/seed_data/cutdown_data.xlsx
+++ b/priv/repo/seed_data/cutdown_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Delta\VSCodeProjects\Elixir\hunt_cutdown\priv\repo\seed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6D85AC-C3B0-4479-B6AD-F32586786471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152BE567-39BE-45B2-8AD3-D1A797355D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{CFAAF1BE-5F0A-4BF6-8FA8-DA56725A7889}"/>
+    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15990" xr2:uid="{CFAAF1BE-5F0A-4BF6-8FA8-DA56725A7889}"/>
   </bookViews>
   <sheets>
     <sheet name="weapons" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="263">
   <si>
     <t>id</t>
   </si>
@@ -57,9 +57,6 @@
     <t>cost</t>
   </si>
   <si>
-    <t>Empty</t>
-  </si>
-  <si>
     <t>Combat Axe</t>
   </si>
   <si>
@@ -286,10 +283,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Empty</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>size</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -627,13 +620,6 @@
     <t>weapon_winfield_m1876_centennial</t>
   </si>
   <si>
-    <t>weapon_empty</t>
-  </si>
-  <si>
-    <t>weapon_empty</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>weapon_bornheim_no_3_extended</t>
   </si>
   <si>
@@ -830,10 +816,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>tool_empty</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Aid</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -859,13 +841,6 @@
   </si>
   <si>
     <t>Trap</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>consumable_empty</t>
-  </si>
-  <si>
-    <t>consumable_empty</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -994,10 +969,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{556468E7-C156-4C1D-A904-E9509552ADF0}" name="テーブル1" displayName="テーブル1" ref="A1:G76" totalsRowShown="0">
-  <autoFilter ref="A1:G76" xr:uid="{556468E7-C156-4C1D-A904-E9509552ADF0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G76">
-    <sortCondition ref="A1:A76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{556468E7-C156-4C1D-A904-E9509552ADF0}" name="テーブル1" displayName="テーブル1" ref="A1:G75" totalsRowShown="0">
+  <autoFilter ref="A1:G75" xr:uid="{556468E7-C156-4C1D-A904-E9509552ADF0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G75">
+    <sortCondition ref="A1:A75"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9DC508E2-45A8-48F1-982F-B4DAFEC7311D}" name="id"/>
@@ -1030,10 +1005,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{53520963-85B2-497E-96B8-108502AAACB4}" name="テーブル13" displayName="テーブル13" ref="A1:C31" totalsRowShown="0">
-  <autoFilter ref="A1:C31" xr:uid="{53520963-85B2-497E-96B8-108502AAACB4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C30">
-    <sortCondition ref="A1:A30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{53520963-85B2-497E-96B8-108502AAACB4}" name="テーブル13" displayName="テーブル13" ref="A1:C30" totalsRowShown="0">
+  <autoFilter ref="A1:C30" xr:uid="{53520963-85B2-497E-96B8-108502AAACB4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C29">
+    <sortCondition ref="A1:A29"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2668D639-FFC3-46C5-9100-673C129D42F2}" name="id"/>
@@ -1045,8 +1020,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4C6BC4AF-CCEC-4CEA-BF7F-A1AC9C4F903C}" name="テーブル3" displayName="テーブル3" ref="A1:E20" totalsRowShown="0">
-  <autoFilter ref="A1:E20" xr:uid="{4C6BC4AF-CCEC-4CEA-BF7F-A1AC9C4F903C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4C6BC4AF-CCEC-4CEA-BF7F-A1AC9C4F903C}" name="テーブル3" displayName="テーブル3" ref="A1:E19" totalsRowShown="0">
+  <autoFilter ref="A1:E19" xr:uid="{4C6BC4AF-CCEC-4CEA-BF7F-A1AC9C4F903C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3FB9CF39-4A4A-476D-AC75-148000FBD738}" name="id"/>
     <tableColumn id="2" xr3:uid="{3D97AE95-4DF1-4C4E-8A7F-4D5A410E6A3C}" name="full_name"/>
@@ -1059,10 +1034,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96026C8F-0053-4D3A-8650-D6BB03E17072}" name="テーブル36" displayName="テーブル36" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10" xr:uid="{96026C8F-0053-4D3A-8650-D6BB03E17072}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C10">
-    <sortCondition ref="A1:A10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{96026C8F-0053-4D3A-8650-D6BB03E17072}" name="テーブル36" displayName="テーブル36" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{96026C8F-0053-4D3A-8650-D6BB03E17072}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C9">
+    <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E8B1D6A7-5C21-44B6-824C-083C4E6FDF35}" name="id"/>
@@ -1074,10 +1049,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6544C1EF-2F02-4561-A44E-9FA21494489D}" name="テーブル35" displayName="テーブル35" ref="A1:E23" totalsRowShown="0">
-  <autoFilter ref="A1:E23" xr:uid="{6544C1EF-2F02-4561-A44E-9FA21494489D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
-    <sortCondition ref="E1:E23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6544C1EF-2F02-4561-A44E-9FA21494489D}" name="テーブル35" displayName="テーブル35" ref="A1:E22" totalsRowShown="0">
+  <autoFilter ref="A1:E22" xr:uid="{6544C1EF-2F02-4561-A44E-9FA21494489D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+    <sortCondition ref="E1:E22"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7D421A52-B484-47CE-B10D-9CE2404B800F}" name="id"/>
@@ -1091,10 +1066,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{249C3092-A0DD-41C3-9BE6-0929CF500C56}" name="テーブル357" displayName="テーブル357" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{249C3092-A0DD-41C3-9BE6-0929CF500C56}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C7">
-    <sortCondition ref="A1:A7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{249C3092-A0DD-41C3-9BE6-0929CF500C56}" name="テーブル357" displayName="テーブル357" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{249C3092-A0DD-41C3-9BE6-0929CF500C56}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C6">
+    <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{21D2B571-8DF3-490E-A7F7-50C1B43915C3}" name="id"/>
@@ -1402,10 +1377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BA7AA3-F1C6-4BE5-AC87-BE482E377C23}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75:C75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1433,30 +1408,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>199</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -1467,19 +1442,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1490,19 +1465,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>306</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1513,19 +1488,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>224</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1536,19 +1511,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1559,19 +1534,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1582,19 +1557,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1605,19 +1580,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1628,19 +1603,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1651,19 +1626,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1674,19 +1649,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1697,19 +1672,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1720,19 +1695,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>600</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1743,19 +1718,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15">
         <v>750</v>
       </c>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1766,19 +1741,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16">
         <v>790</v>
       </c>
       <c r="E16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1789,22 +1764,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1812,42 +1787,42 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D18">
-        <v>35</v>
+        <v>397</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D19">
-        <v>397</v>
+        <v>437</v>
       </c>
       <c r="E19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1858,19 +1833,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1881,42 +1856,42 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D21">
-        <v>422</v>
+        <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1927,19 +1902,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D23">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1950,7 +1925,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
@@ -1959,10 +1934,10 @@
         <v>45</v>
       </c>
       <c r="D24">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1973,19 +1948,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1996,19 +1971,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2019,19 +1994,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D27">
-        <v>164</v>
+        <v>490</v>
       </c>
       <c r="E27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -2042,19 +2017,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D28">
-        <v>490</v>
+        <v>1250</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2065,19 +2040,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D29">
-        <v>1250</v>
+        <v>540</v>
       </c>
       <c r="E29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2088,19 +2063,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D30">
-        <v>540</v>
+        <v>290</v>
       </c>
       <c r="E30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2111,19 +2086,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D31">
-        <v>290</v>
+        <v>350</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2134,19 +2109,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D32">
-        <v>350</v>
+        <v>310</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2157,19 +2132,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D33">
-        <v>310</v>
+        <v>550</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2180,19 +2155,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>550</v>
+        <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2203,19 +2178,19 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2226,19 +2201,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D36">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2249,7 +2224,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="B37" t="s">
         <v>29</v>
@@ -2258,10 +2233,10 @@
         <v>29</v>
       </c>
       <c r="D37">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2272,19 +2247,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D38">
-        <v>80</v>
+        <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2295,7 +2270,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="B39" t="s">
         <v>52</v>
@@ -2304,10 +2279,10 @@
         <v>52</v>
       </c>
       <c r="D39">
-        <v>155</v>
+        <v>211</v>
       </c>
       <c r="E39" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -2318,19 +2293,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D40">
-        <v>211</v>
+        <v>29</v>
       </c>
       <c r="E40" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2341,19 +2316,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D41">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2364,19 +2339,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="D42">
-        <v>53</v>
+        <v>1015</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -2387,19 +2362,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="D43">
-        <v>1015</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2410,19 +2385,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D44">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2433,19 +2408,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D45">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2456,19 +2431,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D46">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2479,19 +2454,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D47">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="E47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2502,7 +2477,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
@@ -2511,10 +2486,10 @@
         <v>49</v>
       </c>
       <c r="D48">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="E48" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2525,7 +2500,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -2534,10 +2509,10 @@
         <v>50</v>
       </c>
       <c r="D49">
-        <v>150</v>
+        <v>199</v>
       </c>
       <c r="E49" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -2548,19 +2523,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D50">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -2571,7 +2546,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="B51" t="s">
         <v>55</v>
@@ -2580,10 +2555,10 @@
         <v>55</v>
       </c>
       <c r="D51">
-        <v>188</v>
+        <v>223</v>
       </c>
       <c r="E51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2594,19 +2569,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D52">
-        <v>223</v>
+        <v>164</v>
       </c>
       <c r="E52" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2617,19 +2592,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D53">
-        <v>164</v>
+        <v>38</v>
       </c>
       <c r="E53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2640,19 +2615,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D54">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2663,19 +2638,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D55">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E55" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2686,7 +2661,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B56" t="s">
         <v>18</v>
@@ -2695,10 +2670,10 @@
         <v>18</v>
       </c>
       <c r="D56">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E56" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2709,7 +2684,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B57" t="s">
         <v>19</v>
@@ -2718,10 +2693,10 @@
         <v>19</v>
       </c>
       <c r="D57">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E57" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -2732,19 +2707,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D58">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2755,19 +2730,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
-        <v>172</v>
+        <v>207</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C59" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D59">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="E59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2778,19 +2753,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D60">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="E60" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2801,19 +2776,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C61" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D61">
-        <v>130</v>
+        <v>309</v>
       </c>
       <c r="E61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2824,19 +2799,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D62">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="E62" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2847,19 +2822,19 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
-        <v>213</v>
+        <v>172</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D63">
-        <v>289</v>
+        <v>75</v>
       </c>
       <c r="E63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2870,7 +2845,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="B64" t="s">
         <v>32</v>
@@ -2879,10 +2854,10 @@
         <v>32</v>
       </c>
       <c r="D64">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E64" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2893,19 +2868,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B65" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D65">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="E65" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2916,19 +2891,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D66">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E66" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2939,19 +2914,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B67" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D67">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="E67" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2962,19 +2937,19 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="B68" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D68">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="E68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2985,19 +2960,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D69">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E69" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -3008,19 +2983,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D70">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E70" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -3031,19 +3006,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D71">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E71" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -3054,19 +3029,19 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D72">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E72" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -3077,19 +3052,19 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B73" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D73">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E73" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -3100,19 +3075,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>174</v>
       </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C74" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D74">
-        <v>39</v>
+        <v>277</v>
       </c>
       <c r="E74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -3123,7 +3098,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="B75" t="s">
         <v>61</v>
@@ -3135,35 +3110,12 @@
         <v>277</v>
       </c>
       <c r="E75" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F75">
         <v>1</v>
       </c>
       <c r="G75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>223</v>
-      </c>
-      <c r="B76" t="s">
-        <v>62</v>
-      </c>
-      <c r="C76" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76">
-        <v>277</v>
-      </c>
-      <c r="E76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
         <v>0</v>
       </c>
     </row>
@@ -3181,7 +3133,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3206,41 +3158,41 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D3">
         <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3254,10 +3206,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BD4DE2-0449-4D45-A184-1A352F0E2A91}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3268,7 +3220,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3279,332 +3231,321 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3618,10 +3559,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A40719F-CCE4-44A7-B269-AD8980D5404D}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3646,89 +3587,89 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>243</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>100</v>
@@ -3736,33 +3677,33 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>101</v>
@@ -3770,169 +3711,169 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>231</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>237</v>
+        <v>107</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
         <v>108</v>
@@ -3940,36 +3881,19 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>234</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3983,10 +3907,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20EB0D6-A63A-4D0E-9024-0E89563F89B3}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4008,101 +3932,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>239</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>244</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -4116,10 +4029,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BFA5AD-CA52-4628-BE8A-F6A3094FEB18}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4144,114 +4057,114 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2">
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D4">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D6">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D7">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>247</v>
       </c>
       <c r="B8" t="s">
         <v>126</v>
@@ -4260,44 +4173,44 @@
         <v>126</v>
       </c>
       <c r="D8">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>254</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
@@ -4311,15 +4224,15 @@
         <v>119</v>
       </c>
       <c r="D11">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>248</v>
       </c>
       <c r="B12" t="s">
         <v>121</v>
@@ -4328,44 +4241,44 @@
         <v>121</v>
       </c>
       <c r="D12">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D13">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D14">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
@@ -4379,15 +4292,15 @@
         <v>125</v>
       </c>
       <c r="D15">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>249</v>
       </c>
       <c r="B16" t="s">
         <v>127</v>
@@ -4396,100 +4309,100 @@
         <v>127</v>
       </c>
       <c r="D16">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>258</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D21">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
         <v>122</v>
@@ -4498,27 +4411,10 @@
         <v>122</v>
       </c>
       <c r="D22">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23">
-        <v>25</v>
-      </c>
-      <c r="E23" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -4532,10 +4428,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D404AD-48DD-4B7F-BC1F-812A5D25AD44}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4558,68 +4454,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>241</v>
-      </c>
-      <c r="B7" t="s">
-        <v>249</v>
-      </c>
-      <c r="C7" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>